<commit_message>
Modification de la doc (Mis a jour du planning detail)
</commit_message>
<xml_diff>
--- a/Version 5/Documentation/planification_detaillee.xlsx
+++ b/Version 5/Documentation/planification_detaillee.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="315" windowWidth="13350" windowHeight="13965" tabRatio="500"/>
+    <workbookView xWindow="13590" yWindow="540" windowWidth="13350" windowHeight="13965" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -761,7 +761,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modifier utilisateur 75% done
</commit_message>
<xml_diff>
--- a/Version 5/Documentation/planification_detaillee.xlsx
+++ b/Version 5/Documentation/planification_detaillee.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13590" yWindow="540" windowWidth="13350" windowHeight="13965" tabRatio="500"/>
+    <workbookView xWindow="11850" yWindow="-45" windowWidth="13350" windowHeight="13965" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
   <si>
     <t>Fonctionnalités</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Afficher fontaines</t>
   </si>
   <si>
-    <t>Accepter fontaines</t>
-  </si>
-  <si>
     <t>H = 45mn</t>
   </si>
   <si>
@@ -104,6 +101,12 @@
   </si>
   <si>
     <t>Geolocalisation</t>
+  </si>
+  <si>
+    <t>Gestion Admin</t>
+  </si>
+  <si>
+    <t>Gestion Utilisateur</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,12 +179,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF660066"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,7 +336,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -366,52 +363,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -758,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -774,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3">
         <v>14.11</v>
@@ -797,40 +791,40 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="8">
         <v>4</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -839,14 +833,14 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="22">
+        <v>13</v>
+      </c>
+      <c r="B4" s="21">
         <v>0.5</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24" t="s">
-        <v>11</v>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -855,14 +849,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="22">
+        <v>14</v>
+      </c>
+      <c r="B5" s="21">
         <v>0.5</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="25" t="s">
-        <v>10</v>
+      <c r="C5" s="22"/>
+      <c r="D5" s="24" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -878,7 +872,7 @@
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -894,7 +888,7 @@
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -910,7 +904,7 @@
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -927,17 +921,17 @@
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="8">
         <v>4</v>
@@ -945,7 +939,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="12"/>
@@ -963,13 +957,13 @@
       <c r="E11" s="12"/>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B12" s="8">
         <v>4</v>
@@ -977,42 +971,56 @@
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="F12" s="9"/>
+      <c r="H12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="8">
+        <v>4</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="9"/>
+      <c r="H13" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>